<commit_message>
fix to run data
</commit_message>
<xml_diff>
--- a/resources/data/30/Lập trình Web 2025/issue.xlsx
+++ b/resources/data/30/Lập trình Web 2025/issue.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="92">
   <si>
     <t>issue_name</t>
   </si>
@@ -89,9 +89,15 @@
     <t>3438c873-bc50-42c4-a598-1ed31761fe23</t>
   </si>
   <si>
+    <t>BLOCKED</t>
+  </si>
+  <si>
     <t>Phân tích đối tượng khách hàng sách</t>
   </si>
   <si>
+    <t>TRIVIAL</t>
+  </si>
+  <si>
     <t>Issue thêm sprint 1</t>
   </si>
   <si>
@@ -161,37 +167,127 @@
     <t>Vẽ sơ bộ sơ đồ use case của hệ thống</t>
   </si>
   <si>
+    <t>Xây dựng sơ đồ use-case ban đầu</t>
+  </si>
+  <si>
+    <t>d909ec23-e3b8-473c-8b53-b0dd10e5cb4a</t>
+  </si>
+  <si>
+    <t>Khảo sát thị trường mỹ phẩm &amp; chăm sóc da</t>
+  </si>
+  <si>
+    <t>Nghiên cứu tính năng đánh giá &amp; gợi ý sản phẩm</t>
+  </si>
+  <si>
+    <t>Khảo sát thị trường và đối thủ</t>
+  </si>
+  <si>
+    <t>dc9af886-7862-4815-9876-037e5440de12</t>
+  </si>
+  <si>
+    <t>Thu thập yêu cầu tính năng</t>
+  </si>
+  <si>
+    <t>f27d5a34-ecc1-4c32-8fd9-44615cbbed19</t>
+  </si>
+  <si>
+    <t>Nghiên cứu yêu cầu về thông tin chi tiết cây</t>
+  </si>
+  <si>
+    <t>Khảo sát các loại cây cảnh phổ biến &amp; nhu cầu</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho quản lý người tham dự &amp; đăng ký</t>
+  </si>
+  <si>
+    <t>d74cdee3-a4fc-44b4-bd90-1e53bec5cad1</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho sự kiện &amp; loại vé</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho thanh toán &amp; hóa đơn</t>
+  </si>
+  <si>
+    <t>Chuẩn hóa CSDL và tối ưu truy vấn ban đầu</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho danh mục sách &amp; tác giả</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho tính năng đánh giá &amp; đề xuất</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho nhà hàng &amp; menu</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho đơn hàng &amp; giao hàng</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho người bán &amp; cộng đồng</t>
+  </si>
+  <si>
+    <t>Nạp dữ liệu cho CSDL</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho sản phẩm tùy chỉnh &amp; biến thể</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho sản phẩm thể thao &amp; thuộc tính</t>
+  </si>
+  <si>
+    <t>Rà soát ERD</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho tính năng đề xuất sản phẩm</t>
+  </si>
+  <si>
+    <t>Chuẩn hóa CSDL và tối ưu hóa truy vấn</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho bảo hành và hỗ trợ khách hàng</t>
+  </si>
+  <si>
+    <t>Xây dựng ERD cho thông số kỹ thuật sản phẩm</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho sơ đồ ghế &amp; vé</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho người dùng &amp; phân quyền</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho phim &amp; lịch chiếu</t>
+  </si>
+  <si>
     <t>MINOR</t>
   </si>
   <si>
-    <t>Xây dựng sơ đồ use-case ban đầu</t>
-  </si>
-  <si>
-    <t>d909ec23-e3b8-473c-8b53-b0dd10e5cb4a</t>
-  </si>
-  <si>
-    <t>Khảo sát thị trường mỹ phẩm &amp; chăm sóc da</t>
-  </si>
-  <si>
-    <t>Nghiên cứu tính năng đánh giá &amp; gợi ý sản phẩm</t>
-  </si>
-  <si>
-    <t>Khảo sát thị trường và đối thủ</t>
-  </si>
-  <si>
-    <t>dc9af886-7862-4815-9876-037e5440de12</t>
-  </si>
-  <si>
-    <t>Thu thập yêu cầu tính năng</t>
-  </si>
-  <si>
-    <t>f27d5a34-ecc1-4c32-8fd9-44615cbbed19</t>
-  </si>
-  <si>
-    <t>Nghiên cứu yêu cầu về thông tin chi tiết cây</t>
-  </si>
-  <si>
-    <t>Khảo sát các loại cây cảnh phổ biến &amp; nhu cầu</t>
+    <t>Thiết kế ERD cho giỏ hàng, đơn hàng và thanh toán</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho đánh giá &amp; gợi ý cá nhân hóa</t>
+  </si>
+  <si>
+    <t>Rà soát và thống nhất naming convention CSDL</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho sản phẩm mỹ phẩm &amp; loại da/tóc</t>
+  </si>
+  <si>
+    <t>Chuẩn hóa cơ sở dữ liệu &amp; tối ưu</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho người dùng &amp; đơn hàng</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho sản phẩm &amp; danh mục</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho cây cảnh &amp; vật tư</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD cho hướng dẫn chăm sóc &amp; bài viết</t>
   </si>
 </sst>
 </file>
@@ -236,7 +332,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:P72"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -339,7 +435,7 @@
         <v>1.0</v>
       </c>
       <c r="P2" t="n" s="0">
-        <v>0.2727272727272727</v>
+        <v>0.36363636363636365</v>
       </c>
     </row>
     <row r="3">
@@ -418,7 +514,7 @@
         <v>0.0</v>
       </c>
       <c r="I4" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J4" t="n" s="0">
         <v>0.0</v>
@@ -456,7 +552,7 @@
         <v>19</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F5" t="n" s="0">
         <v>0.0</v>
@@ -465,7 +561,7 @@
         <v>1.0</v>
       </c>
       <c r="H5" t="n" s="0">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="I5" t="n" s="0">
         <v>1.0</v>
@@ -480,7 +576,7 @@
         <v>0.0</v>
       </c>
       <c r="M5" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N5" t="n" s="0">
         <v>0.0</v>
@@ -489,12 +585,12 @@
         <v>1.0</v>
       </c>
       <c r="P5" t="n" s="0">
-        <v>0.0</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>24</v>
@@ -506,7 +602,7 @@
         <v>19</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F6" t="n" s="0">
         <v>0.0</v>
@@ -515,10 +611,10 @@
         <v>1.0</v>
       </c>
       <c r="H6" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I6" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="J6" t="n" s="0">
         <v>0.0</v>
@@ -530,7 +626,7 @@
         <v>0.0</v>
       </c>
       <c r="M6" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N6" t="n" s="0">
         <v>0.0</v>
@@ -544,7 +640,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s" s="0">
         <v>24</v>
@@ -553,10 +649,10 @@
         <v>18</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F7" t="n" s="0">
         <v>0.0</v>
@@ -565,7 +661,7 @@
         <v>1.0</v>
       </c>
       <c r="H7" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I7" t="n" s="0">
         <v>0.0</v>
@@ -594,7 +690,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s" s="0">
         <v>24</v>
@@ -615,7 +711,7 @@
         <v>1.0</v>
       </c>
       <c r="H8" t="n" s="0">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="I8" t="n" s="0">
         <v>1.0</v>
@@ -636,7 +732,7 @@
         <v>0.0</v>
       </c>
       <c r="O8" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P8" t="n" s="0">
         <v>0.0</v>
@@ -644,10 +740,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>18</v>
@@ -665,10 +761,10 @@
         <v>1.0</v>
       </c>
       <c r="H9" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I9" t="n" s="0">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="J9" t="n" s="0">
         <v>0.0</v>
@@ -697,7 +793,7 @@
         <v>22</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>18</v>
@@ -715,10 +811,10 @@
         <v>1.0</v>
       </c>
       <c r="H10" t="n" s="0">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="I10" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J10" t="n" s="0">
         <v>0.0</v>
@@ -744,10 +840,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>18</v>
@@ -765,7 +861,7 @@
         <v>1.0</v>
       </c>
       <c r="H11" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I11" t="n" s="0">
         <v>1.0</v>
@@ -789,7 +885,7 @@
         <v>0.0</v>
       </c>
       <c r="P11" t="n" s="0">
-        <v>0.45454545454545453</v>
+        <v>0.8181818181818182</v>
       </c>
     </row>
     <row r="12">
@@ -797,7 +893,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s" s="0">
         <v>18</v>
@@ -844,10 +940,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s" s="0">
         <v>18</v>
@@ -894,10 +990,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s" s="0">
         <v>35</v>
-      </c>
-      <c r="B14" t="s" s="0">
-        <v>33</v>
       </c>
       <c r="C14" t="s" s="0">
         <v>18</v>
@@ -906,7 +1002,7 @@
         <v>19</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F14" t="n" s="0">
         <v>0.0</v>
@@ -944,10 +1040,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s" s="0">
         <v>18</v>
@@ -994,10 +1090,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s" s="0">
         <v>18</v>
@@ -1047,7 +1143,7 @@
         <v>22</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s" s="0">
         <v>18</v>
@@ -1094,10 +1190,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s" s="0">
         <v>18</v>
@@ -1144,10 +1240,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>18</v>
@@ -1168,7 +1264,7 @@
         <v>0.0</v>
       </c>
       <c r="I19" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J19" t="n" s="0">
         <v>0.0</v>
@@ -1194,10 +1290,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s" s="0">
         <v>18</v>
@@ -1206,7 +1302,7 @@
         <v>19</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F20" t="n" s="0">
         <v>0.0</v>
@@ -1218,7 +1314,7 @@
         <v>0.0</v>
       </c>
       <c r="I20" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J20" t="n" s="0">
         <v>0.0</v>
@@ -1230,7 +1326,7 @@
         <v>0.0</v>
       </c>
       <c r="M20" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N20" t="n" s="0">
         <v>0.0</v>
@@ -1244,10 +1340,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s" s="0">
         <v>43</v>
-      </c>
-      <c r="B21" t="s" s="0">
-        <v>41</v>
       </c>
       <c r="C21" t="s" s="0">
         <v>18</v>
@@ -1268,7 +1364,7 @@
         <v>0.0</v>
       </c>
       <c r="I21" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="J21" t="n" s="0">
         <v>0.0</v>
@@ -1294,10 +1390,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s" s="0">
         <v>18</v>
@@ -1306,7 +1402,7 @@
         <v>19</v>
       </c>
       <c r="E22" t="s" s="0">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F22" t="n" s="0">
         <v>0.0</v>
@@ -1318,7 +1414,7 @@
         <v>0.0</v>
       </c>
       <c r="I22" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J22" t="n" s="0">
         <v>0.0</v>
@@ -1330,13 +1426,13 @@
         <v>0.0</v>
       </c>
       <c r="M22" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N22" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="O22" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P22" t="n" s="0">
         <v>0.0</v>
@@ -1344,10 +1440,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s" s="0">
         <v>18</v>
@@ -1356,7 +1452,7 @@
         <v>19</v>
       </c>
       <c r="E23" t="s" s="0">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F23" t="n" s="0">
         <v>0.0</v>
@@ -1380,7 +1476,7 @@
         <v>0.0</v>
       </c>
       <c r="M23" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N23" t="n" s="0">
         <v>0.0</v>
@@ -1394,10 +1490,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s" s="0">
         <v>18</v>
@@ -1447,7 +1543,7 @@
         <v>22</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s" s="0">
         <v>18</v>
@@ -1494,10 +1590,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s" s="0">
         <v>48</v>
-      </c>
-      <c r="B26" t="s" s="0">
-        <v>46</v>
       </c>
       <c r="C26" t="s" s="0">
         <v>18</v>
@@ -1506,7 +1602,7 @@
         <v>19</v>
       </c>
       <c r="E26" t="s" s="0">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="F26" t="n" s="0">
         <v>0.0</v>
@@ -1518,7 +1614,7 @@
         <v>0.0</v>
       </c>
       <c r="I26" t="n" s="0">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="J26" t="n" s="0">
         <v>0.0</v>
@@ -1530,7 +1626,7 @@
         <v>0.0</v>
       </c>
       <c r="M26" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N26" t="n" s="0">
         <v>0.0</v>
@@ -1544,10 +1640,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s" s="0">
         <v>18</v>
@@ -1556,7 +1652,7 @@
         <v>19</v>
       </c>
       <c r="E27" t="s" s="0">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F27" t="n" s="0">
         <v>0.0</v>
@@ -1597,7 +1693,7 @@
         <v>22</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s" s="0">
         <v>18</v>
@@ -1618,7 +1714,7 @@
         <v>0.0</v>
       </c>
       <c r="I28" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J28" t="n" s="0">
         <v>0.0</v>
@@ -1644,10 +1740,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s" s="0">
         <v>52</v>
-      </c>
-      <c r="B29" t="s" s="0">
-        <v>51</v>
       </c>
       <c r="C29" t="s" s="0">
         <v>18</v>
@@ -1694,10 +1790,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s" s="0">
         <v>18</v>
@@ -1744,10 +1840,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s" s="0">
         <v>18</v>
@@ -1756,7 +1852,7 @@
         <v>19</v>
       </c>
       <c r="E31" t="s" s="0">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F31" t="n" s="0">
         <v>0.0</v>
@@ -1765,7 +1861,7 @@
         <v>1.0</v>
       </c>
       <c r="H31" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I31" t="n" s="0">
         <v>1.0</v>
@@ -1780,7 +1876,7 @@
         <v>0.0</v>
       </c>
       <c r="M31" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N31" t="n" s="0">
         <v>0.0</v>
@@ -1794,10 +1890,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="B32" t="s" s="0">
         <v>56</v>
-      </c>
-      <c r="B32" t="s" s="0">
-        <v>55</v>
       </c>
       <c r="C32" t="s" s="0">
         <v>18</v>
@@ -1806,7 +1902,7 @@
         <v>19</v>
       </c>
       <c r="E32" t="s" s="0">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F32" t="n" s="0">
         <v>0.0</v>
@@ -1815,10 +1911,10 @@
         <v>1.0</v>
       </c>
       <c r="H32" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I32" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J32" t="n" s="0">
         <v>0.0</v>
@@ -1830,7 +1926,7 @@
         <v>0.0</v>
       </c>
       <c r="M32" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N32" t="n" s="0">
         <v>0.0</v>
@@ -1847,7 +1943,7 @@
         <v>22</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s" s="0">
         <v>18</v>
@@ -1865,7 +1961,7 @@
         <v>1.0</v>
       </c>
       <c r="H33" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I33" t="n" s="0">
         <v>1.0</v>
@@ -1894,10 +1990,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="B34" t="s" s="0">
         <v>58</v>
-      </c>
-      <c r="B34" t="s" s="0">
-        <v>57</v>
       </c>
       <c r="C34" t="s" s="0">
         <v>18</v>
@@ -1915,7 +2011,7 @@
         <v>1.0</v>
       </c>
       <c r="H34" t="n" s="0">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="I34" t="n" s="0">
         <v>0.0</v>
@@ -1944,10 +2040,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s" s="0">
         <v>18</v>
@@ -1965,7 +2061,7 @@
         <v>1.0</v>
       </c>
       <c r="H35" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I35" t="n" s="0">
         <v>1.0</v>
@@ -1990,6 +2086,1856 @@
       </c>
       <c r="P35" t="n" s="0">
         <v>0.45454545454545453</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D36" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E36" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G36" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H36" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P36" t="n" s="0">
+        <v>0.6363636363636364</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D37" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E37" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G37" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H37" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I37" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P37" t="n" s="0">
+        <v>0.9090909090909091</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D38" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E38" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G38" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H38" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O38" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="P38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D39" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E39" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G39" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H39" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="I39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O39" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="P39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D40" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E40" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G40" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H40" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I40" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P40" t="n" s="0">
+        <v>0.6363636363636364</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D41" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E41" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G41" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H41" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="I41" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P41" t="n" s="0">
+        <v>0.45454545454545453</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D42" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E42" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G42" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H42" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I42" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P42" t="n" s="0">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E43" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G43" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H43" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P43" t="n" s="0">
+        <v>0.4166666666666667</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E44" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G44" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H44" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I44" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M44" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="N44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O44" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="P44" t="n" s="0">
+        <v>0.18181818181818182</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E45" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G45" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P45" t="n" s="0">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E46" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G46" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I46" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E47" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G47" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I47" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M47" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="N47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O47" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="P47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E48" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G48" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H48" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I48" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P48" t="n" s="0">
+        <v>0.2727272727272727</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E49" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G49" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H49" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I49" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O49" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="P49" t="n" s="0">
+        <v>0.2727272727272727</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E50" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G50" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H50" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O50" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="P50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E51" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G51" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H51" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O51" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="P51" t="n" s="0">
+        <v>0.45454545454545453</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D52" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E52" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F52" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G52" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H52" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I52" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J52" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K52" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L52" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M52" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N52" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O52" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P52" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D53" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E53" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F53" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G53" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H53" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I53" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J53" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K53" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L53" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M53" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N53" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O53" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P53" t="n" s="0">
+        <v>0.2727272727272727</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D54" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E54" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F54" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G54" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H54" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I54" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J54" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K54" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L54" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M54" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N54" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O54" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P54" t="n" s="0">
+        <v>0.5555555555555556</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D55" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E55" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F55" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G55" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H55" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I55" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="J55" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K55" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L55" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M55" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N55" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O55" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P55" t="n" s="0">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="B56" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D56" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E56" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F56" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G56" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H56" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I56" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J56" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K56" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L56" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M56" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N56" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O56" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P56" t="n" s="0">
+        <v>0.5555555555555556</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="B57" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C57" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D57" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E57" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F57" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G57" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H57" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I57" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J57" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K57" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L57" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M57" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N57" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O57" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P57" t="n" s="0">
+        <v>0.18181818181818182</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="B58" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D58" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E58" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F58" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G58" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H58" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I58" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J58" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K58" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L58" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M58" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N58" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O58" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="P58" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="B59" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C59" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D59" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E59" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F59" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G59" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H59" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I59" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J59" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K59" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L59" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M59" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N59" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O59" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="P59" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="B60" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C60" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D60" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E60" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F60" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G60" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H60" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I60" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J60" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K60" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L60" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M60" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N60" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O60" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="P60" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="B61" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C61" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D61" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E61" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="F61" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G61" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H61" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I61" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J61" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K61" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L61" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M61" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="N61" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O61" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P61" t="n" s="0">
+        <v>0.18181818181818182</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="B62" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C62" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D62" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E62" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F62" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G62" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H62" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I62" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J62" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K62" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L62" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M62" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N62" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O62" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="P62" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="B63" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C63" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D63" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E63" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F63" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G63" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H63" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I63" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J63" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K63" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L63" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M63" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N63" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O63" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P63" t="n" s="0">
+        <v>0.45454545454545453</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="B64" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C64" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D64" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E64" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F64" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G64" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H64" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I64" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J64" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K64" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L64" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M64" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N64" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O64" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P64" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B65" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C65" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D65" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E65" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F65" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G65" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H65" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I65" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J65" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K65" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L65" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M65" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N65" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O65" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P65" t="n" s="0">
+        <v>0.7272727272727273</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C66" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D66" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E66" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F66" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G66" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H66" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I66" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J66" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K66" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L66" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M66" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N66" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O66" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="P66" t="n" s="0">
+        <v>0.7272727272727273</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="B67" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C67" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D67" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E67" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F67" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G67" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H67" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I67" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J67" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K67" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L67" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M67" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N67" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O67" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P67" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B68" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C68" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D68" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E68" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F68" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G68" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H68" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="I68" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J68" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K68" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L68" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M68" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N68" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O68" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P68" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C69" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D69" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E69" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F69" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G69" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H69" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I69" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J69" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K69" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L69" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M69" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N69" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O69" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P69" t="n" s="0">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B70" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="C70" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D70" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E70" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F70" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G70" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H70" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I70" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J70" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K70" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L70" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M70" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="N70" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O70" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="P70" t="n" s="0">
+        <v>0.6363636363636364</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="B71" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="C71" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D71" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E71" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F71" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G71" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H71" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I71" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J71" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K71" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L71" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M71" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N71" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O71" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P71" t="n" s="0">
+        <v>0.6363636363636364</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="B72" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="C72" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D72" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E72" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F72" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G72" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H72" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="I72" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J72" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K72" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L72" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M72" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N72" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O72" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="P72" t="n" s="0">
+        <v>0.6363636363636364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>